<commit_message>
CU Administrar Cliente y la interfaz alumno
Se realizó el CU Administrar Cliente y la interfaz alumno
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_3 Registro.xlsx
+++ b/Documentos/Tareas/Iteración_3 Registro.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Documents\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymu\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBD8D89-F0F8-4EB0-B2A2-A8624F3396EA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -869,10 +870,10 @@
   <dimension ref="B1:BW52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z10" sqref="Z10"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1599,7 @@
         <v>43</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="G8" s="22">
         <v>1</v>
@@ -1681,67 +1682,69 @@
         <v>1</v>
       </c>
       <c r="AT8" s="23"/>
-      <c r="AU8" s="23"/>
+      <c r="AU8" s="23">
+        <v>1</v>
+      </c>
       <c r="AV8" s="23">
         <f t="shared" ref="AV8" si="41">AS8-AU8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW8" s="23"/>
       <c r="AX8" s="23"/>
       <c r="AY8" s="23">
         <f t="shared" ref="AY8" si="42">AV8-AX8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ8" s="23"/>
       <c r="BA8" s="23"/>
       <c r="BB8" s="23">
         <f t="shared" ref="BB8:BB33" si="43">AY8-BA8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC8" s="23"/>
       <c r="BD8" s="23"/>
       <c r="BE8" s="23">
         <f t="shared" ref="BE8:BE33" si="44">BB8-BD8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF8" s="23"/>
       <c r="BG8" s="23"/>
       <c r="BH8" s="23">
         <f t="shared" ref="BH8:BH33" si="45">BE8-BG8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI8" s="23"/>
       <c r="BJ8" s="23"/>
       <c r="BK8" s="23">
         <f t="shared" ref="BK8:BK33" si="46">BH8-BJ8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL8" s="23"/>
       <c r="BM8" s="23"/>
       <c r="BN8" s="23">
         <f t="shared" ref="BN8:BN33" si="47">BK8-BM8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO8" s="23"/>
       <c r="BP8" s="23"/>
       <c r="BQ8" s="23">
         <f t="shared" ref="BQ8:BQ33" si="48">BN8-BP8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR8" s="23"/>
       <c r="BS8" s="23"/>
       <c r="BT8" s="23">
         <f t="shared" ref="BT8:BT33" si="49">BQ8-BS8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU8" s="23"/>
       <c r="BV8" s="23">
         <f t="shared" ref="BV8:BV33" si="50">H8+K8+N8+Q8+T8+W8+Z8+AC8+AF8+AI8+AL8+AO8+AR8+AU8+AX8+BA8+BD8+BG8+BJ8+BM8+BP8+BS8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW8" s="23">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:75" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2072,7 +2075,7 @@
         <v>43</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="G11" s="22">
         <v>2</v>
@@ -2107,115 +2110,121 @@
         <v>2</v>
       </c>
       <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
+      <c r="W11" s="23">
+        <v>2</v>
+      </c>
       <c r="X11" s="23">
         <f t="shared" si="56"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="23"/>
       <c r="Z11" s="23"/>
       <c r="AA11" s="23">
         <f t="shared" si="57"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
+      <c r="AC11" s="23">
+        <v>1</v>
+      </c>
       <c r="AD11" s="23">
         <f t="shared" si="58"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
+      <c r="AF11" s="23">
+        <v>2</v>
+      </c>
       <c r="AG11" s="23">
         <f t="shared" si="59"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AH11" s="23"/>
       <c r="AI11" s="23"/>
       <c r="AJ11" s="23">
         <f t="shared" si="60"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AK11" s="23"/>
       <c r="AL11" s="23"/>
       <c r="AM11" s="23">
         <f t="shared" si="61"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AN11" s="23"/>
       <c r="AO11" s="23"/>
       <c r="AP11" s="23">
         <f t="shared" si="62"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AQ11" s="23"/>
       <c r="AR11" s="23"/>
       <c r="AS11" s="23">
         <f t="shared" si="63"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AT11" s="23"/>
       <c r="AU11" s="23"/>
       <c r="AV11" s="23">
         <f t="shared" si="64"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AW11" s="23"/>
       <c r="AX11" s="23"/>
       <c r="AY11" s="23">
         <f t="shared" si="65"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AZ11" s="23"/>
       <c r="BA11" s="23"/>
       <c r="BB11" s="23">
         <f t="shared" si="43"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="BC11" s="23"/>
       <c r="BD11" s="23"/>
       <c r="BE11" s="23">
         <f t="shared" si="44"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="BF11" s="23"/>
       <c r="BG11" s="23"/>
       <c r="BH11" s="23">
         <f t="shared" si="45"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="BI11" s="23"/>
       <c r="BJ11" s="23"/>
       <c r="BK11" s="23">
         <f t="shared" si="46"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="BL11" s="23"/>
       <c r="BM11" s="23"/>
       <c r="BN11" s="23">
         <f t="shared" si="47"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="BO11" s="23"/>
       <c r="BP11" s="23"/>
       <c r="BQ11" s="23">
         <f t="shared" si="48"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="BR11" s="23"/>
       <c r="BS11" s="23"/>
       <c r="BT11" s="23">
         <f t="shared" si="49"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="BU11" s="23"/>
       <c r="BV11" s="23">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BW11" s="23">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="12" spans="2:75" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2856,7 +2865,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="G16" s="22">
         <v>2</v>
@@ -2969,37 +2978,39 @@
         <v>2</v>
       </c>
       <c r="BI16" s="23"/>
-      <c r="BJ16" s="23"/>
+      <c r="BJ16" s="23">
+        <v>0.5</v>
+      </c>
       <c r="BK16" s="23">
         <f t="shared" si="46"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BL16" s="23"/>
       <c r="BM16" s="23"/>
       <c r="BN16" s="23">
         <f t="shared" si="47"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BO16" s="23"/>
       <c r="BP16" s="23"/>
       <c r="BQ16" s="23">
         <f t="shared" si="48"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BR16" s="23"/>
       <c r="BS16" s="23"/>
       <c r="BT16" s="23">
         <f t="shared" si="49"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BU16" s="23"/>
       <c r="BV16" s="23">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BW16" s="23">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="2:75" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3281,37 +3292,39 @@
         <v>2</v>
       </c>
       <c r="BI18" s="23"/>
-      <c r="BJ18" s="23"/>
+      <c r="BJ18" s="23">
+        <v>0.5</v>
+      </c>
       <c r="BK18" s="23">
         <f t="shared" si="46"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BL18" s="23"/>
       <c r="BM18" s="23"/>
       <c r="BN18" s="23">
         <f t="shared" si="47"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BO18" s="23"/>
       <c r="BP18" s="23"/>
       <c r="BQ18" s="23">
         <f t="shared" si="48"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BR18" s="23"/>
       <c r="BS18" s="23"/>
       <c r="BT18" s="23">
         <f t="shared" si="49"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BU18" s="23"/>
       <c r="BV18" s="23">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BW18" s="23">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="2:75" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3960,7 +3973,7 @@
         <v>43</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="G23" s="22">
         <v>3</v>
@@ -4073,37 +4086,39 @@
         <v>3</v>
       </c>
       <c r="BI23" s="23"/>
-      <c r="BJ23" s="23"/>
+      <c r="BJ23" s="23">
+        <v>2</v>
+      </c>
       <c r="BK23" s="23">
         <f t="shared" si="46"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BL23" s="23"/>
       <c r="BM23" s="23"/>
       <c r="BN23" s="23">
         <f t="shared" si="47"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BO23" s="23"/>
       <c r="BP23" s="23"/>
       <c r="BQ23" s="23">
         <f t="shared" si="48"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BR23" s="23"/>
       <c r="BS23" s="23"/>
       <c r="BT23" s="23">
         <f t="shared" si="49"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BU23" s="23"/>
       <c r="BV23" s="23">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BW23" s="23">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:75" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -7056,6 +7071,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AI4:AJ4"/>
     <mergeCell ref="BV4:BW4"/>
     <mergeCell ref="AO4:AP4"/>
     <mergeCell ref="AR4:AS4"/>
@@ -7068,17 +7094,6 @@
     <mergeCell ref="BM4:BN4"/>
     <mergeCell ref="BP4:BQ4"/>
     <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AI4:AJ4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>